<commit_message>
Completed analysis of a semester and also fixed backlog handling
</commit_message>
<xml_diff>
--- a/test_files/backlog_test_data.xlsx
+++ b/test_files/backlog_test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\Projects\mini_Project\new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\Projects\mini_Project\new\result_analysis\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8C2BA2-6BFC-4C98-86F2-5CE0E9C8C117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D517CF0-FA8D-4B94-B04C-F7B0E7487DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2CD0994-6D25-49C1-8714-EF1D270803CB}"/>
   </bookViews>
@@ -568,6 +568,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -598,27 +619,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1124719-4E9C-4116-A121-57BFE3CDB4B7}">
   <dimension ref="A1:AZ322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="AV16" sqref="AV16"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2975,60 +2975,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="25"/>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="25"/>
-      <c r="AZ1" s="25"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
     </row>
     <row r="2" spans="1:52" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3043,31 +3043,31 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="26"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
@@ -3082,528 +3082,528 @@
       <c r="AU2" s="1"/>
     </row>
     <row r="3" spans="1:52" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="27"/>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="27"/>
-      <c r="AI3" s="27"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="27"/>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="27"/>
-      <c r="AR3" s="27"/>
-      <c r="AS3" s="27"/>
-      <c r="AT3" s="27"/>
-      <c r="AU3" s="27"/>
-      <c r="AV3" s="27"/>
-      <c r="AW3" s="27"/>
-      <c r="AX3" s="27"/>
-      <c r="AY3" s="27"/>
-      <c r="AZ3" s="27"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10"/>
     </row>
     <row r="4" spans="1:52" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27"/>
-      <c r="AX4" s="27"/>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
+      <c r="AV4" s="10"/>
+      <c r="AW4" s="10"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="10"/>
+      <c r="AZ4" s="10"/>
     </row>
     <row r="5" spans="1:52" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="27"/>
-      <c r="AM5" s="27"/>
-      <c r="AN5" s="27"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="27"/>
-      <c r="AR5" s="27"/>
-      <c r="AS5" s="27"/>
-      <c r="AT5" s="27"/>
-      <c r="AU5" s="27"/>
-      <c r="AV5" s="27"/>
-      <c r="AW5" s="27"/>
-      <c r="AX5" s="27"/>
-      <c r="AY5" s="27"/>
-      <c r="AZ5" s="27"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10"/>
+      <c r="AX5" s="10"/>
+      <c r="AY5" s="10"/>
+      <c r="AZ5" s="10"/>
     </row>
     <row r="6" spans="1:52" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="27"/>
-      <c r="AF6" s="27"/>
-      <c r="AG6" s="27"/>
-      <c r="AH6" s="27"/>
-      <c r="AI6" s="27"/>
-      <c r="AJ6" s="27"/>
-      <c r="AK6" s="27"/>
-      <c r="AL6" s="27"/>
-      <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="27"/>
-      <c r="AQ6" s="27"/>
-      <c r="AR6" s="27"/>
-      <c r="AS6" s="27"/>
-      <c r="AT6" s="27"/>
-      <c r="AU6" s="27"/>
-      <c r="AV6" s="27"/>
-      <c r="AW6" s="27"/>
-      <c r="AX6" s="27"/>
-      <c r="AY6" s="27"/>
-      <c r="AZ6" s="27"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
     </row>
     <row r="7" spans="1:52" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="21"/>
-      <c r="AN7" s="21"/>
-      <c r="AO7" s="21"/>
-      <c r="AP7" s="21"/>
-      <c r="AQ7" s="21"/>
-      <c r="AR7" s="21"/>
-      <c r="AS7" s="21"/>
-      <c r="AT7" s="21"/>
-      <c r="AU7" s="21"/>
-      <c r="AV7" s="21"/>
-      <c r="AW7" s="21"/>
-      <c r="AX7" s="21"/>
-      <c r="AY7" s="21"/>
-      <c r="AZ7" s="21"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="13"/>
+      <c r="AZ7" s="13"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="10" t="s">
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="10" t="s">
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="10" t="s">
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="10" t="s">
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="10" t="s">
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="10" t="s">
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="19"/>
+      <c r="AL8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="12"/>
-      <c r="AQ8" s="10" t="s">
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="19"/>
+      <c r="AQ8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="AR8" s="11"/>
-      <c r="AS8" s="11"/>
-      <c r="AT8" s="11"/>
-      <c r="AU8" s="12"/>
-      <c r="AV8" s="10" t="s">
+      <c r="AR8" s="18"/>
+      <c r="AS8" s="18"/>
+      <c r="AT8" s="18"/>
+      <c r="AU8" s="19"/>
+      <c r="AV8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AW8" s="11"/>
-      <c r="AX8" s="11"/>
-      <c r="AY8" s="11"/>
-      <c r="AZ8" s="12"/>
+      <c r="AW8" s="18"/>
+      <c r="AX8" s="18"/>
+      <c r="AY8" s="18"/>
+      <c r="AZ8" s="19"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="14"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="15"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
-      <c r="AO9" s="14"/>
-      <c r="AP9" s="15"/>
-      <c r="AQ9" s="13"/>
-      <c r="AR9" s="14"/>
-      <c r="AS9" s="14"/>
-      <c r="AT9" s="14"/>
-      <c r="AU9" s="15"/>
-      <c r="AV9" s="13"/>
-      <c r="AW9" s="14"/>
-      <c r="AX9" s="14"/>
-      <c r="AY9" s="14"/>
-      <c r="AZ9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="21"/>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="21"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="21"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="21"/>
+      <c r="AN9" s="21"/>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="22"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="21"/>
+      <c r="AS9" s="21"/>
+      <c r="AT9" s="21"/>
+      <c r="AU9" s="22"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="21"/>
+      <c r="AX9" s="21"/>
+      <c r="AY9" s="21"/>
+      <c r="AZ9" s="22"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="13"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AO10" s="14"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="13"/>
-      <c r="AR10" s="14"/>
-      <c r="AS10" s="14"/>
-      <c r="AT10" s="14"/>
-      <c r="AU10" s="15"/>
-      <c r="AV10" s="13"/>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="14"/>
-      <c r="AY10" s="14"/>
-      <c r="AZ10" s="15"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="21"/>
+      <c r="AK10" s="22"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="21"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="21"/>
+      <c r="AP10" s="22"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="21"/>
+      <c r="AS10" s="21"/>
+      <c r="AT10" s="21"/>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="20"/>
+      <c r="AW10" s="21"/>
+      <c r="AX10" s="21"/>
+      <c r="AY10" s="21"/>
+      <c r="AZ10" s="22"/>
     </row>
     <row r="11" spans="1:52" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="17"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="18"/>
-      <c r="AL11" s="16"/>
-      <c r="AM11" s="17"/>
-      <c r="AN11" s="17"/>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="18"/>
-      <c r="AQ11" s="16"/>
-      <c r="AR11" s="17"/>
-      <c r="AS11" s="17"/>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="18"/>
-      <c r="AV11" s="16"/>
-      <c r="AW11" s="17"/>
-      <c r="AX11" s="17"/>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="18"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="25"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="24"/>
+      <c r="AJ11" s="24"/>
+      <c r="AK11" s="25"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="24"/>
+      <c r="AN11" s="24"/>
+      <c r="AO11" s="24"/>
+      <c r="AP11" s="25"/>
+      <c r="AQ11" s="23"/>
+      <c r="AR11" s="24"/>
+      <c r="AS11" s="24"/>
+      <c r="AT11" s="24"/>
+      <c r="AU11" s="25"/>
+      <c r="AV11" s="23"/>
+      <c r="AW11" s="24"/>
+      <c r="AX11" s="24"/>
+      <c r="AY11" s="24"/>
+      <c r="AZ11" s="25"/>
     </row>
     <row r="12" spans="1:52" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -4148,7 +4148,7 @@
         <v>0</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="AA15" s="3">
         <v>0</v>
@@ -4246,7 +4246,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -4419,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -19630,28 +19630,24 @@
       <c r="AU293" s="9"/>
     </row>
     <row r="322" spans="1:52" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A322" s="19" t="s">
+      <c r="A322" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B322" s="19"/>
-      <c r="C322" s="19"/>
-      <c r="AU322" s="20" t="s">
+      <c r="B322" s="26"/>
+      <c r="C322" s="26"/>
+      <c r="AU322" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="AV322" s="20"/>
-      <c r="AW322" s="20"/>
-      <c r="AX322" s="20"/>
-      <c r="AY322" s="20"/>
-      <c r="AZ322" s="20"/>
+      <c r="AV322" s="27"/>
+      <c r="AW322" s="27"/>
+      <c r="AX322" s="27"/>
+      <c r="AY322" s="27"/>
+      <c r="AZ322" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A6:AZ6"/>
-    <mergeCell ref="A1:AZ1"/>
-    <mergeCell ref="M2:AI2"/>
-    <mergeCell ref="A3:AZ3"/>
-    <mergeCell ref="A4:AZ4"/>
-    <mergeCell ref="A5:AZ5"/>
+    <mergeCell ref="A322:C322"/>
+    <mergeCell ref="AU322:AZ322"/>
     <mergeCell ref="A7:AZ7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B12"/>
@@ -19665,8 +19661,12 @@
     <mergeCell ref="AL8:AP11"/>
     <mergeCell ref="AQ8:AU11"/>
     <mergeCell ref="AV8:AZ11"/>
-    <mergeCell ref="A322:C322"/>
-    <mergeCell ref="AU322:AZ322"/>
+    <mergeCell ref="A6:AZ6"/>
+    <mergeCell ref="A1:AZ1"/>
+    <mergeCell ref="M2:AI2"/>
+    <mergeCell ref="A3:AZ3"/>
+    <mergeCell ref="A4:AZ4"/>
+    <mergeCell ref="A5:AZ5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>